<commit_message>
Add unit and integration tests for ceramic zone normalization and wall calculations
- Implement tests for ceramic zone normalization in `test_ceramic_zone_normalizer.py` to ensure correct perimeter and area calculations.
- Create comprehensive unit tests for data models in `test_models.py`, covering Room, Opening, Wall, FinishItem, and CeramicZone classes.
- Add tests for UnifiedCalculator in `test_unified_calculator.py`, validating wall gross area calculations, plaster, paint, and baseboard metrics.
- Introduce integration tests in `test_wall_ceramic_integration.py` to verify that wall edits correctly update ceramic zone metrics and handle opening deductions.
</commit_message>
<xml_diff>
--- a/test_export.xlsx
+++ b/test_export.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -29,8 +29,8 @@
     <font>
       <name val="Segoe UI"/>
       <b val="1"/>
-      <color rgb="001F4E78"/>
-      <sz val="18"/>
+      <color rgb="00FFFFFF"/>
+      <sz val="11"/>
     </font>
     <font>
       <name val="Segoe UI"/>
@@ -39,16 +39,10 @@
     </font>
     <font>
       <name val="Segoe UI"/>
-      <b val="1"/>
-      <color rgb="00FFFFFF"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Segoe UI"/>
       <sz val="10"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
@@ -59,12 +53,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="001F4E78"/>
         <bgColor rgb="001F4E78"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00BDD7EE"/>
-        <bgColor rgb="00BDD7EE"/>
       </patternFill>
     </fill>
   </fills>
@@ -94,25 +82,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="2" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -478,36 +461,21 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="B2:D17"/>
   <sheetViews>
     <sheetView showGridLines="0" rightToLeft="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="4" customWidth="1" min="1" max="1"/>
-    <col width="29" customWidth="1" min="2" max="2"/>
-    <col width="8" customWidth="1" min="3" max="3"/>
-    <col width="8" customWidth="1" min="4" max="4"/>
-  </cols>
   <sheetData>
-    <row r="1"/>
     <row r="2">
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>ملخص كميات المشروع</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>تاريخ التقرير: 2025-12-21</t>
-        </is>
-      </c>
-    </row>
-    <row r="4"/>
+          <t>ملخص الكميات (SSOT Verified)</t>
+        </is>
+      </c>
+    </row>
     <row r="5">
       <c r="B5" s="2" t="inlineStr">
         <is>
@@ -517,16 +485,11 @@
       <c r="C5" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>غرفة</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>مساحة الأرضيات الإجمالية</t>
+          <t>مساحات الأرضيات (إجمالي)</t>
         </is>
       </c>
       <c r="C6" s="3" t="n">
@@ -541,7 +504,7 @@
     <row r="7">
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>أعمال الزريقة (لياسة)</t>
+          <t>أعمال الزريقة (SSOT)</t>
         </is>
       </c>
       <c r="C7" s="3" t="n">
@@ -556,11 +519,11 @@
     <row r="8">
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>أعمال الدهان</t>
+          <t>أعمال الدهان (SSOT)</t>
         </is>
       </c>
       <c r="C8" s="3" t="n">
-        <v>44.9</v>
+        <v>46.4</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -571,11 +534,11 @@
     <row r="9">
       <c r="B9" s="2" t="inlineStr">
         <is>
-          <t>سيراميك الجدران</t>
+          <t>سيراميك الجدران (SSOT)</t>
         </is>
       </c>
       <c r="C9" s="3" t="n">
-        <v>27</v>
+        <v>25.5</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -586,7 +549,7 @@
     <row r="10">
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>سيراميك الأرضيات</t>
+          <t>سيراميك الأرضيات (SSOT)</t>
         </is>
       </c>
       <c r="C10" s="3" t="n">
@@ -601,11 +564,11 @@
     <row r="11">
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>سيراميك (إجمالي صافي)</t>
+          <t>إجمالي السيراميك (SSOT)</t>
         </is>
       </c>
       <c r="C11" s="3" t="n">
-        <v>27</v>
+        <v>25.5</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -616,7 +579,7 @@
     <row r="12">
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>نعلات (وزرات)</t>
+          <t>نعلات (SSOT)</t>
         </is>
       </c>
       <c r="C12" s="3" t="n">
@@ -631,13 +594,68 @@
     <row r="13">
       <c r="B13" s="2" t="inlineStr">
         <is>
-          <t>حجر (إطارات فتحات)</t>
+          <t>حجر/أطر (SSOT)</t>
         </is>
       </c>
       <c r="C13" s="3" t="n">
         <v>5.2</v>
       </c>
       <c r="D13" t="inlineStr">
+        <is>
+          <t>م.ط</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>مساحة الفتحات (أبواب+شبابيك)</t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>م²</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>عدد الفتحات (أبواب+شبابيك)</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" s="2" t="inlineStr">
+        <is>
+          <t>بلاط الأرضيات (دفتر البنود)</t>
+        </is>
+      </c>
+      <c r="C16" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>م²</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" s="2" t="inlineStr">
+        <is>
+          <t>نعلات (دفتر البنود)</t>
+        </is>
+      </c>
+      <c r="C17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" t="inlineStr">
         <is>
           <t>م.ط</t>
         </is>
@@ -654,7 +672,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView showGridLines="0" rightToLeft="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -662,22 +680,24 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="5" customWidth="1" min="1" max="1"/>
-    <col width="14" customWidth="1" min="2" max="2"/>
-    <col width="14" customWidth="1" min="3" max="3"/>
-    <col width="10" customWidth="1" min="4" max="4"/>
-    <col width="11" customWidth="1" min="5" max="5"/>
-    <col width="14" customWidth="1" min="6" max="6"/>
-    <col width="16" customWidth="1" min="7" max="7"/>
-    <col width="22" customWidth="1" min="8" max="8"/>
-    <col width="30" customWidth="1" min="9" max="9"/>
-    <col width="22" customWidth="1" min="10" max="10"/>
-    <col width="30" customWidth="1" min="11" max="11"/>
-    <col width="15" customWidth="1" min="12" max="12"/>
-    <col width="22" customWidth="1" min="13" max="13"/>
-    <col width="23" customWidth="1" min="14" max="14"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="20" customWidth="1" min="9" max="9"/>
+    <col width="20" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="11" max="11"/>
+    <col width="20" customWidth="1" min="12" max="12"/>
+    <col width="20" customWidth="1" min="13" max="13"/>
+    <col width="20" customWidth="1" min="14" max="14"/>
     <col width="20" customWidth="1" min="15" max="15"/>
-    <col width="17" customWidth="1" min="16" max="16"/>
+    <col width="20" customWidth="1" min="16" max="16"/>
+    <col width="20" customWidth="1" min="17" max="17"/>
+    <col width="20" customWidth="1" min="18" max="18"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -688,77 +708,87 @@
       </c>
       <c r="B1" s="4" t="inlineStr">
         <is>
-          <t>اسم الغرفة</t>
+          <t>الغرفة</t>
         </is>
       </c>
       <c r="C1" s="4" t="inlineStr">
         <is>
-          <t>نوع الغرفة</t>
+          <t>النوع</t>
         </is>
       </c>
       <c r="D1" s="4" t="inlineStr">
         <is>
-          <t>الطابق</t>
+          <t>المحيط</t>
         </is>
       </c>
       <c r="E1" s="4" t="inlineStr">
         <is>
-          <t>الأبعاد</t>
+          <t>ارتفاع الجدار</t>
         </is>
       </c>
       <c r="F1" s="4" t="inlineStr">
         <is>
-          <t>المحيط (م)</t>
+          <t>مساحة الأرضية</t>
         </is>
       </c>
       <c r="G1" s="4" t="inlineStr">
         <is>
-          <t>الارتفاع (م)</t>
+          <t>جدران قائمة</t>
         </is>
       </c>
       <c r="H1" s="4" t="inlineStr">
         <is>
-          <t>مساحة الأرضية (م²)</t>
+          <t>خصم فتحات</t>
         </is>
       </c>
       <c r="I1" s="4" t="inlineStr">
         <is>
-          <t>مساحة الجدران القائمة (م²)</t>
+          <t>جدران صافية</t>
         </is>
       </c>
       <c r="J1" s="4" t="inlineStr">
         <is>
-          <t>مساحة الفتحات (م²)</t>
+          <t>زريقة جدران</t>
         </is>
       </c>
       <c r="K1" s="4" t="inlineStr">
         <is>
-          <t>مساحة الجدران الصافية (م²)</t>
+          <t>زريقة سقف</t>
         </is>
       </c>
       <c r="L1" s="4" t="inlineStr">
         <is>
-          <t>نعلات (م.ط)</t>
+          <t>دهان جدران</t>
         </is>
       </c>
       <c r="M1" s="4" t="inlineStr">
         <is>
-          <t>سيراميك جدران (م²)</t>
+          <t>دهان سقف</t>
         </is>
       </c>
       <c r="N1" s="4" t="inlineStr">
         <is>
-          <t>سيراميك أرضيات (م²)</t>
+          <t>سيراميك جدران</t>
         </is>
       </c>
       <c r="O1" s="4" t="inlineStr">
         <is>
-          <t>سيراميك سقف (م²)</t>
+          <t>سيراميك أرضيات</t>
         </is>
       </c>
       <c r="P1" s="4" t="inlineStr">
         <is>
-          <t>ملاحظات</t>
+          <t>سيراميك سقف</t>
+        </is>
+      </c>
+      <c r="Q1" s="4" t="inlineStr">
+        <is>
+          <t>نعلات</t>
+        </is>
+      </c>
+      <c r="R1" s="4" t="inlineStr">
+        <is>
+          <t>حجر/أطر</t>
         </is>
       </c>
     </row>
@@ -766,97 +796,61 @@
       <c r="A2" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="inlineStr">
+      <c r="B2" s="6" t="inlineStr">
         <is>
           <t>غرفة 1</t>
         </is>
       </c>
-      <c r="C2" s="5" t="inlineStr">
+      <c r="C2" s="6" t="inlineStr">
         <is>
           <t>[Not Set]</t>
         </is>
       </c>
       <c r="D2" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="E2" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="G2" s="5" t="n">
+        <v>54</v>
+      </c>
+      <c r="H2" s="5" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="I2" s="5" t="n">
+        <v>51.9</v>
+      </c>
+      <c r="J2" s="5" t="n">
+        <v>51.9</v>
+      </c>
+      <c r="K2" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="L2" s="5" t="n">
+        <v>26.4</v>
+      </c>
+      <c r="M2" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="N2" s="5" t="n">
+        <v>25.5</v>
+      </c>
+      <c r="O2" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="E2" s="5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F2" s="6" t="n">
-        <v>18</v>
-      </c>
-      <c r="G2" s="6" t="n">
-        <v>3</v>
-      </c>
-      <c r="H2" s="6" t="n">
-        <v>20</v>
-      </c>
-      <c r="I2" s="6" t="n">
-        <v>54</v>
-      </c>
-      <c r="J2" s="6" t="n">
-        <v>2.1</v>
-      </c>
-      <c r="K2" s="6" t="n">
-        <v>51.9</v>
-      </c>
-      <c r="L2" s="6" t="n">
+      <c r="P2" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="M2" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N2" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="P2" s="5" t="inlineStr">
-        <is>
-          <t>شكل غير منتظم</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="7" t="inlineStr"/>
-      <c r="B3" s="7" t="inlineStr">
-        <is>
-          <t>الإجمالي</t>
-        </is>
-      </c>
-      <c r="C3" s="8" t="n"/>
-      <c r="D3" s="8" t="n"/>
-      <c r="E3" s="8" t="n"/>
-      <c r="F3" s="8" t="n"/>
-      <c r="G3" s="8" t="n"/>
-      <c r="H3" s="9" t="n">
-        <v>20</v>
-      </c>
-      <c r="I3" s="9" t="n">
-        <v>54</v>
-      </c>
-      <c r="J3" s="9" t="n">
-        <v>2.1</v>
-      </c>
-      <c r="K3" s="9" t="n">
-        <v>51.9</v>
-      </c>
-      <c r="L3" s="9" t="n">
-        <v>17</v>
-      </c>
-      <c r="M3" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="N3" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="O3" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="P3" s="8" t="n"/>
+      <c r="R2" s="5" t="n">
+        <v>5.2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
feat: Enhance ceramic calculation logic and add comprehensive tests
- Unified height calculation logic for ceramic zones across all presets.
- Added tests to ensure room quantities persist through to_dict/from_dict methods.
- Implemented detailed tests for physical openings data to prioritize room quantities.
- Created a diagnostic script to analyze ceramic deductions in real projects.
- Developed tests for various scenarios including manual vs quick ceramic height calculations.
- Improved handling of wall heights in rooms with mixed wall segment heights.
- Added documentation for ceramic button enhancements and their usage.
</commit_message>
<xml_diff>
--- a/test_export.xlsx
+++ b/test_export.xlsx
@@ -461,7 +461,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:D17"/>
+  <dimension ref="B2:D18"/>
   <sheetViews>
     <sheetView showGridLines="0" rightToLeft="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -564,11 +564,11 @@
     <row r="11">
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>إجمالي السيراميك (SSOT)</t>
+          <t>سيراميك الأسقف (SSOT)</t>
         </is>
       </c>
       <c r="C11" s="3" t="n">
-        <v>25.5</v>
+        <v>0</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -579,26 +579,26 @@
     <row r="12">
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>نعلات (SSOT)</t>
+          <t>إجمالي السيراميك (SSOT)</t>
         </is>
       </c>
       <c r="C12" s="3" t="n">
-        <v>17</v>
+        <v>25.5</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>م.ط</t>
+          <t>م²</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="2" t="inlineStr">
         <is>
-          <t>حجر/أطر (SSOT)</t>
+          <t>نعلات (SSOT)</t>
         </is>
       </c>
       <c r="C13" s="3" t="n">
-        <v>5.2</v>
+        <v>0</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -609,53 +609,73 @@
     <row r="14">
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>مساحة الفتحات (أبواب+شبابيك)</t>
+          <t>حجر/أطر (مجموع الغرف)</t>
         </is>
       </c>
       <c r="C14" s="3" t="n">
-        <v>2.1</v>
+        <v>5.2</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>م²</t>
+          <t>م.ط</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="2" t="inlineStr">
         <is>
-          <t>عدد الفتحات (أبواب+شبابيك)</t>
+          <t>مساحة الفتحات (أبواب+شبابيك)</t>
         </is>
       </c>
       <c r="C15" s="3" t="n">
-        <v>1</v>
+        <v>2.1</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>م²</t>
+        </is>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="2" t="inlineStr">
         <is>
-          <t>بلاط الأرضيات (دفتر البنود)</t>
+          <t>عدد الفتحات (أبواب+شبابيك)</t>
         </is>
       </c>
       <c r="C16" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>م²</t>
+          <t>قطعة</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="B17" s="2" t="inlineStr">
         <is>
-          <t>نعلات (دفتر البنود)</t>
+          <t>بلاط الأرضيات (دفتر البنود)</t>
         </is>
       </c>
       <c r="C17" s="3" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="inlineStr">
+        <is>
+          <t>م²</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" s="2" t="inlineStr">
+        <is>
+          <t>نعلات (دفتر البنود)</t>
+        </is>
+      </c>
+      <c r="C18" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" t="inlineStr">
         <is>
           <t>م.ط</t>
         </is>
@@ -672,7 +692,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView showGridLines="0" rightToLeft="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -698,6 +718,7 @@
     <col width="20" customWidth="1" min="16" max="16"/>
     <col width="20" customWidth="1" min="17" max="17"/>
     <col width="20" customWidth="1" min="18" max="18"/>
+    <col width="20" customWidth="1" min="19" max="19"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -791,6 +812,11 @@
           <t>حجر/أطر</t>
         </is>
       </c>
+      <c r="S1" s="4" t="inlineStr">
+        <is>
+          <t>ملاحظات النعلات</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="5" t="n">
@@ -846,10 +872,15 @@
         <v>0</v>
       </c>
       <c r="Q2" s="5" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="R2" s="5" t="n">
         <v>5.2</v>
+      </c>
+      <c r="S2" s="6" t="inlineStr">
+        <is>
+          <t>ملغى (يوجد سيراميك جدران)</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>